<commit_message>
doc(plan/strategie de test); feat(script de deploiement); chore(JDT)
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_NademoYosef.xlsx
+++ b/Doc/Journal-de-Travail_NademoYosef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\Todo-DevOps-Test\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4008031B-B223-482F-84D9-59D0EAB195ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29148F60-3A53-4065-B288-50BD4508EADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>Auteur:</t>
   </si>
@@ -151,6 +151,24 @@
   </si>
   <si>
     <t>Todo-App</t>
+  </si>
+  <si>
+    <t>creation de Github Project pour planification, creation de taches, assignment, prioritarisation,estimation</t>
+  </si>
+  <si>
+    <t>deploiement d'application</t>
+  </si>
+  <si>
+    <t>creation d'un plan tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">creation d'une strategie de tests, </t>
+  </si>
+  <si>
+    <t>mis à jour du journal de travail, tout les points de travail effectué sont noté</t>
+  </si>
+  <si>
+    <t>creation de script de deploiement automatique; install-dependencies-launch</t>
   </si>
 </sst>
 </file>
@@ -1175,13 +1193,13 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2105,16 +2123,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.7</c:v>
+                  <c:v>0.28000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.16</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.3</c:v>
+                  <c:v>0.56000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4303,7 +4321,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4358,7 +4376,7 @@
       <c r="B3" s="88"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>1 heures 40 minutes</v>
+        <v>4 heures 10 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4377,11 +4395,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>40</v>
+        <v>190</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4418,10 +4436,10 @@
     <row r="7" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="61">
         <f>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</f>
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B7" s="26">
-        <v>45898</v>
+        <v>45974</v>
       </c>
       <c r="C7" s="27">
         <v>1</v>
@@ -4442,10 +4460,10 @@
     <row r="8" spans="1:15" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A8" s="62">
         <f>IF(ISBLANK(B8),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B8))</f>
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B8" s="30">
-        <v>45898</v>
+        <v>45974</v>
       </c>
       <c r="C8" s="31"/>
       <c r="D8" s="32">
@@ -4470,16 +4488,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="63" t="str">
+    <row r="9" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="63">
         <f>IF(ISBLANK(B9),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B9))</f>
-        <v/>
-      </c>
-      <c r="B9" s="34"/>
+        <v>47</v>
+      </c>
+      <c r="B9" s="34">
+        <v>45981</v>
+      </c>
       <c r="C9" s="35"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="23"/>
+      <c r="D9" s="36">
+        <v>30</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>36</v>
+      </c>
       <c r="G9" s="40"/>
       <c r="M9" t="s">
         <v>19</v>
@@ -4491,16 +4517,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="62" t="str">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="62">
         <f>IF(ISBLANK(B10),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B10))</f>
-        <v/>
-      </c>
-      <c r="B10" s="30"/>
+        <v>47</v>
+      </c>
+      <c r="B10" s="30">
+        <v>45981</v>
+      </c>
       <c r="C10" s="31"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="23"/>
+      <c r="D10" s="32">
+        <v>30</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>37</v>
+      </c>
       <c r="G10" s="85"/>
       <c r="M10" t="s">
         <v>3</v>
@@ -4512,16 +4546,24 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="63" t="str">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="63">
         <f>IF(ISBLANK(B11),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B11))</f>
-        <v/>
-      </c>
-      <c r="B11" s="34"/>
+        <v>47</v>
+      </c>
+      <c r="B11" s="34">
+        <v>45981</v>
+      </c>
       <c r="C11" s="35"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="23"/>
+      <c r="D11" s="36">
+        <v>35</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>38</v>
+      </c>
       <c r="G11" s="40"/>
       <c r="M11" t="s">
         <v>4</v>
@@ -4534,15 +4576,23 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="62" t="str">
+      <c r="A12" s="62">
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B12))</f>
-        <v/>
-      </c>
-      <c r="B12" s="30"/>
+        <v>47</v>
+      </c>
+      <c r="B12" s="30">
+        <v>45981</v>
+      </c>
       <c r="C12" s="31"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="23"/>
+      <c r="D12" s="32">
+        <v>35</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>39</v>
+      </c>
       <c r="G12" s="85"/>
       <c r="M12" t="s">
         <v>28</v>
@@ -4554,16 +4604,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="63" x14ac:dyDescent="0.25">
-      <c r="A13" s="63" t="str">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="63">
         <f>IF(ISBLANK(B13),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B13))</f>
-        <v/>
-      </c>
-      <c r="B13" s="34"/>
+        <v>47</v>
+      </c>
+      <c r="B13" s="34">
+        <v>45981</v>
+      </c>
       <c r="C13" s="35"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="23"/>
+      <c r="D13" s="36">
+        <v>10</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>41</v>
+      </c>
       <c r="G13" s="84"/>
       <c r="N13">
         <v>6</v>
@@ -4572,16 +4630,24 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="62" t="str">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="62">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="30"/>
+        <v>47</v>
+      </c>
+      <c r="B14" s="30">
+        <v>45981</v>
+      </c>
       <c r="C14" s="31"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="23"/>
+      <c r="D14" s="32">
+        <v>10</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>40</v>
+      </c>
       <c r="G14" s="39"/>
       <c r="N14">
         <v>7</v>
@@ -4590,7 +4656,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="63" t="str">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
         <v/>
@@ -4608,7 +4674,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="62" t="str">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
         <v/>
@@ -4623,7 +4689,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="63" t="str">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
         <v/>
@@ -4668,7 +4734,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="62" t="str">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B20))</f>
         <v/>
@@ -4692,7 +4758,7 @@
       <c r="F21" s="23"/>
       <c r="G21" s="40"/>
     </row>
-    <row r="22" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="62" t="str">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
         <v/>
@@ -4740,7 +4806,7 @@
       <c r="F25" s="23"/>
       <c r="G25" s="84"/>
     </row>
-    <row r="26" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="62" t="str">
         <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B26))</f>
         <v/>
@@ -4788,7 +4854,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="40"/>
     </row>
-    <row r="30" spans="1:15" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="62" t="str">
         <f>IF(ISBLANK(B30),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B30))</f>
         <v/>
@@ -10990,7 +11056,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.7</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11011,11 +11077,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11023,11 +11089,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>0 h 00 min</v>
+        <v>0 h 40 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11085,11 +11151,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>30</v>
+        <v>140</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>140</v>
       </c>
       <c r="E9" s="77" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11097,11 +11163,11 @@
       </c>
       <c r="F9" s="74" t="str">
         <f t="shared" si="1"/>
-        <v>0 h 30 min</v>
+        <v>2 h 20 min</v>
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.3</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11157,22 +11223,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>40</v>
+        <v>190</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>1 h 40 min</v>
+        <v>4 h 10 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>6.9444444444444448E-2</v>
+        <v>0.1736111111111111</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Stratégie de test pour projet «cicd-todo-app »
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_NademoYosef.xlsx
+++ b/Doc/Journal-de-Travail_NademoYosef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\Todo-DevOps-Test\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29148F60-3A53-4065-B288-50BD4508EADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CD04C2-C0DD-4468-9EF7-B4B8A356AEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
   <si>
     <t>Auteur:</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>creation de script de deploiement automatique; install-dependencies-launch</t>
+  </si>
+  <si>
+    <t>mis à jour de README.md pour mieux expliquer les but de projet et les poitns de deploiement</t>
   </si>
 </sst>
 </file>
@@ -1199,7 +1202,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>140</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2123,16 +2126,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.28000000000000003</c:v>
+                  <c:v>0.25925925925925924</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.16</c:v>
+                  <c:v>0.14814814814814814</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.56000000000000005</c:v>
+                  <c:v>0.59259259259259256</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4321,7 +4324,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4376,7 +4379,7 @@
       <c r="B3" s="88"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>4 heures 10 minutes</v>
+        <v>4 heures 30 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4395,11 +4398,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4640,13 +4643,13 @@
       </c>
       <c r="C14" s="31"/>
       <c r="D14" s="32">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E14" s="33" t="s">
         <v>4</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G14" s="39"/>
       <c r="N14">
@@ -4657,15 +4660,23 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="63" t="str">
+      <c r="A15" s="63">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
-        <v/>
-      </c>
-      <c r="B15" s="34"/>
+        <v>47</v>
+      </c>
+      <c r="B15" s="34">
+        <v>45981</v>
+      </c>
       <c r="C15" s="35"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="23"/>
+      <c r="D15" s="36">
+        <v>10</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>40</v>
+      </c>
       <c r="G15" s="40"/>
       <c r="N15">
         <v>8</v>
@@ -11056,7 +11067,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.28000000000000003</v>
+        <v>0.25925925925925924</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11093,7 +11104,7 @@
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.16</v>
+        <v>0.14814814814814814</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11151,11 +11162,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="E9" s="77" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11163,11 +11174,11 @@
       </c>
       <c r="F9" s="74" t="str">
         <f t="shared" si="1"/>
-        <v>2 h 20 min</v>
+        <v>2 h 40 min</v>
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.56000000000000005</v>
+        <v>0.59259259259259256</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11223,22 +11234,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>4 h 10 min</v>
+        <v>4 h 30 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.1736111111111111</v>
+        <v>0.1875</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11282,6 +11293,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11290,15 +11310,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11503,6 +11514,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11511,14 +11530,6 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update documentation files and 1.1	Stratégie de test
Updated Journal-de-Travail, PlanTest, and cicd-todo-app_Rapport documents.
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_NademoYosef.xlsx
+++ b/Doc/Journal-de-Travail_NademoYosef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\Todo-DevOps-Test\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CD04C2-C0DD-4468-9EF7-B4B8A356AEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0577D68C-252A-4BCE-AD9C-B90D0FE9C19C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
   <si>
     <t>Auteur:</t>
   </si>
@@ -162,9 +162,6 @@
     <t>creation d'un plan tests</t>
   </si>
   <si>
-    <t xml:space="preserve">creation d'une strategie de tests, </t>
-  </si>
-  <si>
     <t>mis à jour du journal de travail, tout les points de travail effectué sont noté</t>
   </si>
   <si>
@@ -172,6 +169,15 @@
   </si>
   <si>
     <t>mis à jour de README.md pour mieux expliquer les but de projet et les poitns de deploiement</t>
+  </si>
+  <si>
+    <t>ajout d'un paragraph "Documentation" dans Readme.md</t>
+  </si>
+  <si>
+    <t>creation d'une strategie de tests, avencement</t>
+  </si>
+  <si>
+    <t>modification d'un plan tests, tout sauf Objectif</t>
   </si>
 </sst>
 </file>
@@ -1202,7 +1208,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>160</c:v>
+                  <c:v>205</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2126,16 +2132,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.25925925925925924</c:v>
+                  <c:v>0.22222222222222221</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.14814814814814814</c:v>
+                  <c:v>0.12698412698412698</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.59259259259259256</c:v>
+                  <c:v>0.65079365079365081</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4324,7 +4330,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4379,7 +4385,7 @@
       <c r="B3" s="88"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>4 heures 30 minutes</v>
+        <v>5 heures 15 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4398,11 +4404,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>210</v>
+        <v>255</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>270</v>
+        <v>315</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4559,7 +4565,7 @@
       </c>
       <c r="C11" s="35"/>
       <c r="D11" s="36">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="E11" s="37" t="s">
         <v>4</v>
@@ -4594,7 +4600,7 @@
         <v>4</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="G12" s="85"/>
       <c r="M12" t="s">
@@ -4623,7 +4629,7 @@
         <v>19</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G13" s="84"/>
       <c r="N13">
@@ -4649,7 +4655,7 @@
         <v>4</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G14" s="39"/>
       <c r="N14">
@@ -4675,7 +4681,7 @@
         <v>4</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G15" s="40"/>
       <c r="N15">
@@ -4686,45 +4692,69 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="62" t="str">
+      <c r="A16" s="62">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
-        <v/>
-      </c>
-      <c r="B16" s="30"/>
+        <v>48</v>
+      </c>
+      <c r="B16" s="30">
+        <v>45985</v>
+      </c>
       <c r="C16" s="31"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="23"/>
+      <c r="D16" s="32">
+        <v>15</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>42</v>
+      </c>
       <c r="G16" s="39"/>
       <c r="O16">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="63" t="str">
+      <c r="A17" s="63">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v/>
-      </c>
-      <c r="B17" s="34"/>
+        <v>48</v>
+      </c>
+      <c r="B17" s="34">
+        <v>45985</v>
+      </c>
       <c r="C17" s="35"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="23"/>
+      <c r="D17" s="36">
+        <v>40</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>44</v>
+      </c>
       <c r="G17" s="40"/>
       <c r="O17">
         <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="62" t="str">
+      <c r="A18" s="62">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v/>
-      </c>
-      <c r="B18" s="30"/>
+        <v>48</v>
+      </c>
+      <c r="B18" s="30">
+        <v>45985</v>
+      </c>
       <c r="C18" s="31"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="23"/>
+      <c r="D18" s="32">
+        <v>10</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>39</v>
+      </c>
       <c r="G18" s="39"/>
       <c r="O18">
         <v>50</v>
@@ -11067,7 +11097,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.25925925925925924</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11104,7 +11134,7 @@
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.14814814814814814</v>
+        <v>0.12698412698412698</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11162,11 +11192,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>160</v>
+        <v>205</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>160</v>
+        <v>205</v>
       </c>
       <c r="E9" s="77" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11174,11 +11204,11 @@
       </c>
       <c r="F9" s="74" t="str">
         <f t="shared" si="1"/>
-        <v>2 h 40 min</v>
+        <v>3 h 25 min</v>
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.59259259259259256</v>
+        <v>0.65079365079365081</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11234,22 +11264,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>210</v>
+        <v>255</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>270</v>
+        <v>315</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>4 h 30 min</v>
+        <v>5 h 15 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.1875</v>
+        <v>0.21875</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
rapport( Stratégie et plans de tests) + jdt
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_NademoYosef.xlsx
+++ b/Doc/Journal-de-Travail_NademoYosef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\Todo-DevOps-Test\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0577D68C-252A-4BCE-AD9C-B90D0FE9C19C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F933004-9039-4785-B8F4-44D3B69EC423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
   <si>
     <t>Auteur:</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>modification d'un plan tests, tout sauf Objectif</t>
+  </si>
+  <si>
+    <t>corréction du rapport insertion des partie  Stratégie et plans de tests</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1211,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>205</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2132,16 +2135,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.22222222222222221</c:v>
+                  <c:v>0.20895522388059701</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.12698412698412698</c:v>
+                  <c:v>0.11940298507462686</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.65079365079365081</c:v>
+                  <c:v>0.67164179104477617</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4330,7 +4333,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4385,7 +4388,7 @@
       <c r="B3" s="88"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>5 heures 15 minutes</v>
+        <v>5 heures 35 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4404,11 +4407,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4747,13 +4750,13 @@
       </c>
       <c r="C18" s="31"/>
       <c r="D18" s="32">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E18" s="33" t="s">
         <v>4</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="G18" s="39"/>
       <c r="O18">
@@ -4761,15 +4764,23 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="63" t="str">
+      <c r="A19" s="63">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="34"/>
+        <v>48</v>
+      </c>
+      <c r="B19" s="34">
+        <v>45985</v>
+      </c>
       <c r="C19" s="35"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="23"/>
+      <c r="D19" s="36">
+        <v>10</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>39</v>
+      </c>
       <c r="G19" s="84"/>
       <c r="O19">
         <v>55</v>
@@ -11097,7 +11108,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.22222222222222221</v>
+        <v>0.20895522388059701</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11134,7 +11145,7 @@
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.12698412698412698</v>
+        <v>0.11940298507462686</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11192,11 +11203,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>205</v>
+        <v>225</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>205</v>
+        <v>225</v>
       </c>
       <c r="E9" s="77" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11204,11 +11215,11 @@
       </c>
       <c r="F9" s="74" t="str">
         <f t="shared" si="1"/>
-        <v>3 h 25 min</v>
+        <v>3 h 45 min</v>
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.65079365079365081</v>
+        <v>0.67164179104477617</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11264,22 +11275,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>5 h 15 min</v>
+        <v>5 h 35 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.21875</v>
+        <v>0.2326388888888889</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11323,15 +11334,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11340,6 +11342,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11544,14 +11555,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11560,6 +11563,14 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
doc(Chapitre explicatif de l’usage fait de l’IA dans ce projet)
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_NademoYosef.xlsx
+++ b/Doc/Journal-de-Travail_NademoYosef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\Todo-DevOps-Test\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA926EDE-D7E6-4026-B19D-BBFB3EAAFA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391284A4-32E3-40F9-8D3A-F1DF01C3B360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
   <si>
     <t>Auteur:</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>gitignore</t>
+  </si>
+  <si>
+    <t>Chapitre explicatif de l’usage fait de l’IA dans ce projet</t>
   </si>
 </sst>
 </file>
@@ -1220,7 +1223,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>230</c:v>
+                  <c:v>245</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2144,16 +2147,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.22535211267605634</c:v>
+                  <c:v>0.21621621621621623</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.12676056338028169</c:v>
+                  <c:v>0.12162162162162163</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.647887323943662</c:v>
+                  <c:v>0.66216216216216217</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4342,7 +4345,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4397,7 +4400,7 @@
       <c r="B3" s="88"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>5 heures 55 minutes</v>
+        <v>6 heures 10 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4416,11 +4419,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>295</v>
+        <v>310</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>355</v>
+        <v>370</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4864,9 +4867,15 @@
         <v>45988</v>
       </c>
       <c r="C23" s="35"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="23"/>
+      <c r="D23" s="36">
+        <v>15</v>
+      </c>
+      <c r="E23" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>49</v>
+      </c>
       <c r="G23" s="40"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -11145,7 +11154,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.22535211267605634</v>
+        <v>0.21621621621621623</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11182,7 +11191,7 @@
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.12676056338028169</v>
+        <v>0.12162162162162163</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11240,11 +11249,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>230</v>
+        <v>245</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>230</v>
+        <v>245</v>
       </c>
       <c r="E9" s="77" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11252,11 +11261,11 @@
       </c>
       <c r="F9" s="74" t="str">
         <f t="shared" si="1"/>
-        <v>3 h 50 min</v>
+        <v>4 h 05 min</v>
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.647887323943662</v>
+        <v>0.66216216216216217</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11312,22 +11321,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>295</v>
+        <v>310</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>355</v>
+        <v>370</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>5 h 55 min</v>
+        <v>6 h 10 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.24652777777777779</v>
+        <v>0.25694444444444442</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11371,6 +11380,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11379,15 +11397,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11592,6 +11601,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11600,14 +11617,6 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>